<commit_message>
Smart Music Player v1
Release Note: Integration of Emotion Detection, Music Playlist to VLC or Windows Media Player, Hand Gesture Control (Pause/Play, Increase Volume, Dec Volume, Skip song) .

Future Work: Need to add stop gesture to terminal all programs at once.

Disadvantage: Default Music Player
does not close when program terminated using ctrl+c.
</commit_message>
<xml_diff>
--- a/EmotionLinks.xlsx
+++ b/EmotionLinks.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FY project work\FACE\cv_based_smart_music_player-main\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91128245-AA60-438E-83C1-30646D347A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -39,23 +33,23 @@
     <t>neutral</t>
   </si>
   <si>
-    <t>angry.mp3</t>
-  </si>
-  <si>
-    <t>happy.mp3</t>
-  </si>
-  <si>
-    <t>sad.mp3</t>
-  </si>
-  <si>
-    <t>neutral.mp3</t>
+    <t>.\songs\angry.m3u</t>
+  </si>
+  <si>
+    <t>.\songs\happy.m3u</t>
+  </si>
+  <si>
+    <t>.\songs\neutral.m3u</t>
+  </si>
+  <si>
+    <t>.\songs\sad.m3u</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -162,7 +156,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -214,7 +208,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -408,29 +402,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -452,10 +446,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Emotion and hand gesture window added
problems , Emotion links are incorrect, Single player not playlist player
</commit_message>
<xml_diff>
--- a/EmotionLinks.xlsx
+++ b/EmotionLinks.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FY project work\FACE\cv_based_smart_music_player-main\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91128245-AA60-438E-83C1-30646D347A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -33,23 +39,23 @@
     <t>neutral</t>
   </si>
   <si>
-    <t>.\songs\angry.m3u</t>
-  </si>
-  <si>
-    <t>.\songs\happy.m3u</t>
-  </si>
-  <si>
-    <t>.\songs\neutral.m3u</t>
-  </si>
-  <si>
-    <t>.\songs\sad.m3u</t>
+    <t>angry.mp3</t>
+  </si>
+  <si>
+    <t>happy.mp3</t>
+  </si>
+  <si>
+    <t>sad.mp3</t>
+  </si>
+  <si>
+    <t>neutral.mp3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -208,7 +214,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -402,29 +408,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -446,10 +452,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>